<commit_message>
Version 3.0 - added changing column names
Added function to change the column headers, tweaked to include changes and added tests for new functionality
</commit_message>
<xml_diff>
--- a/data/Test2.xlsx
+++ b/data/Test2.xlsx
@@ -430,12 +430,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Tab 1</t>
+          <t>Column 1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Column 2</t>
+          <t>New Column 2</t>
         </is>
       </c>
     </row>
@@ -445,7 +445,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -455,7 +455,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Values</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -463,35 +463,70 @@
       <c r="A4" t="n">
         <v>4</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>5</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>6</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>7</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>8</v>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>9</v>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -516,12 +551,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Column 1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Column 2</t>
+          <t>New Column 2</t>
         </is>
       </c>
     </row>
@@ -531,7 +566,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -541,7 +576,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Values</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -549,40 +584,80 @@
       <c r="A4" t="n">
         <v>13</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>14</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>15</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>16</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>17</v>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>18</v>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>19</v>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>20</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -607,12 +682,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Sheet 3</t>
+          <t>Column 1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Column 2</t>
+          <t>New Column 2</t>
         </is>
       </c>
     </row>
@@ -622,7 +697,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -632,7 +707,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Values</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -640,40 +715,80 @@
       <c r="A4" t="n">
         <v>23</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>24</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>25</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>26</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>27</v>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>28</v>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>29</v>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>30</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>